<commit_message>
Testing largely done. Code changed so unique works correctly.
This is just before attempting to change the field tracking to being a tag instead of pulled from the CV.
</commit_message>
<xml_diff>
--- a/tests/testing_files/conversion_comparison_type_exact_unique_test.xlsx
+++ b/tests/testing_files/conversion_comparison_type_exact_unique_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparda\Desktop\Moseley Lab\Code\MESSES\tests\testing_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C23E72-E9A3-4C43-89E5-F04547F5401D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26084047-E1FC-481C-A52D-A4C87A54A64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="3120" windowWidth="23640" windowHeight="12015" activeTab="1" xr2:uid="{15FD60AA-0CC8-9F4F-B5F4-2B27D5230080}"/>
+    <workbookView xWindow="3120" yWindow="1830" windowWidth="23640" windowHeight="12015" xr2:uid="{15FD60AA-0CC8-9F4F-B5F4-2B27D5230080}"/>
   </bookViews>
   <sheets>
     <sheet name="#convert" sheetId="6" r:id="rId1"/>
@@ -260,10 +260,10 @@
     <t>#comparison=exact</t>
   </si>
   <si>
-    <t>#measurement.compound.assign</t>
-  </si>
-  <si>
     <t>*#measurement.compound</t>
+  </si>
+  <si>
+    <t>#measurement.assignment.assign</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8067F3B6-BC85-4627-B925-1366E7FE6A62}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -679,7 +679,7 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
         <v>71</v>
@@ -706,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FFFD15-87D9-4AFC-82C0-CA4CE918806E}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -836,7 +836,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>